<commit_message>
fix CIDAR order (#54)
</commit_message>
<xml_diff>
--- a/submissions/kits-murray-cidar-moclo-v1/submission.xlsx
+++ b/submissions/kits-murray-cidar-moclo-v1/submission.xlsx
@@ -32259,8 +32259,8 @@
     </row>
     <row r="2">
       <c r="A2" s="16" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("TRIM(REGEXREPLACE(TEXTJOIN(""|"", FALSE, assembly_grid!1:1), ""\|+$"", """"))"),"upstream_adapter|five_utr|promoter|cds|terminator|downstream_adapter")</f>
-        <v>upstream_adapter|five_utr|promoter|cds|terminator|downstream_adapter</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("TRIM(REGEXREPLACE(TEXTJOIN(""|"", FALSE, assembly_grid!1:1), ""\|+$"", """"))"),"upstream_adapter|promoter|five_utr|cds|terminator|downstream_adapter")</f>
+        <v>upstream_adapter|promoter|five_utr|cds|terminator|downstream_adapter</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>366</v>
@@ -32361,10 +32361,10 @@
         <v>346</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
update CIDAR info (#56)
</commit_message>
<xml_diff>
--- a/submissions/kits-murray-cidar-moclo-v1/submission.xlsx
+++ b/submissions/kits-murray-cidar-moclo-v1/submission.xlsx
@@ -1095,7 +1095,7 @@
     <t xml:space="preserve">CIDAR MoClo Extension </t>
   </si>
   <si>
-    <t>110 extra parts for CIDAR</t>
+    <t>110 extra parts for CIDAR + the compatible original CIDAR parts</t>
   </si>
   <si>
     <t>full_name</t>
@@ -1119,7 +1119,7 @@
     <t>fragment_order</t>
   </si>
   <si>
-    <t>Transcriptional unit</t>
+    <t>Transcriptional Unit</t>
   </si>
   <si>
     <t>5'UTR (with RBS) + promoter + CDS + terminator flanked by Golden Gate adapters</t>
@@ -1128,7 +1128,7 @@
     <t>Pre-composed 5'UTR + promoter + CDS</t>
   </si>
   <si>
-    <t>A level 0 plasmid contains a precomposed 5'UTR + promoter + CDS</t>
+    <t>Transcriptional Unit that uses a level 0 plasmid containing joined 5'UTR + promoter + CDS</t>
   </si>
   <si>
     <t>sequence</t>
@@ -32149,7 +32149,7 @@
     <col customWidth="1" min="1" max="1" width="24.13"/>
     <col customWidth="1" min="2" max="2" width="39.88"/>
     <col customWidth="1" min="3" max="3" width="19.75"/>
-    <col customWidth="1" min="4" max="4" width="36.88"/>
+    <col customWidth="1" min="4" max="4" width="48.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -32243,7 +32243,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="54.63"/>
     <col customWidth="1" min="2" max="2" width="36.88"/>
-    <col customWidth="1" min="3" max="3" width="62.38"/>
+    <col customWidth="1" min="3" max="3" width="67.5"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>